<commit_message>
Co-authored-by: GABRIEL FERNANDO TREJO PAZ <L23212239@tijuana.tecnm.mx>
</commit_message>
<xml_diff>
--- a/uploads/instrumentos_2025-11-20.xlsx
+++ b/uploads/instrumentos_2025-11-20.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -458,9 +458,93 @@
         <v>Laboratorio B</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Vidrios de reloj</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Química</v>
+      </c>
+      <c r="C5" t="str">
+        <v>DISPONIBLE</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Laboratorio 10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Desfibrilador externo automático</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Biomédica</v>
+      </c>
+      <c r="C6" t="str">
+        <v>MANTENIMIENTO</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Laboratorio 31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Portaobjetos</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Química</v>
+      </c>
+      <c r="C7" t="str">
+        <v>DISPONIBLE</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Laboratorio 22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Monitor de signos vitales</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Biomédica</v>
+      </c>
+      <c r="C8" t="str">
+        <v>DISPONIBLE</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Laboratorio 31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Osciloscopio</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Electricidad</v>
+      </c>
+      <c r="C9" t="str">
+        <v>PRESTADO</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Laboratorio 22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Cautín</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Electricidad</v>
+      </c>
+      <c r="C10" t="str">
+        <v>DISPONIBLE</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Laboratorio A</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>